<commit_message>
Update list of bugs found during the tests
</commit_message>
<xml_diff>
--- a/Bugs/Bugs Report.xlsx
+++ b/Bugs/Bugs Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Title</t>
   </si>
@@ -60,6 +60,49 @@
   </si>
   <si>
     <t>Testcafe_Project_E-commerce.</t>
+  </si>
+  <si>
+    <t>Filters_Module: The filters are not working for any product.</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>All browsers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter to the url:  http://automationpractice.com/index.php 
+2. Proceed to any product available.
+3. Proceed to the Catalog section on the left side page. 
+4. Select any filter: color, size, price.
+5. Verify what information is displayed.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The filters applied to any product are  not working when a user selects one or more filters only is displayed a loader icon. </t>
+  </si>
+  <si>
+    <t>The filters applied to any product should be working correctly when a user selects one or more options and the application should display a list of products according the filters selected.</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Filters_Module: The option 'Sort by:' is not working.</t>
+  </si>
+  <si>
+    <t>The option sort by is not working when a user selects any options from the dropdown list. Only is displayed a loader icon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter to the url:  http://automationpractice.com/index.php 
+2. Proceed to any product available.
+3. Proceed to the the sort by option. 
+4. Select any option from the dropdown list.
+5. Verify what information is displayed.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The option sort by should work work correctly when a user selects any options from the dropdown list. </t>
   </si>
 </sst>
 </file>
@@ -278,21 +321,21 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -311,18 +354,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:K17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:K17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="B4:K17"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="#" dataDxfId="10"/>
-    <tableColumn id="2" name="Title" dataDxfId="9"/>
-    <tableColumn id="3" name="Summary" dataDxfId="8"/>
-    <tableColumn id="4" name="Frequency" dataDxfId="7"/>
-    <tableColumn id="5" name="Where(Browser)" dataDxfId="6"/>
-    <tableColumn id="6" name="Steps to Reproduce" dataDxfId="5"/>
-    <tableColumn id="7" name="Actual Result" dataDxfId="4"/>
-    <tableColumn id="8" name="Expected Result" dataDxfId="3"/>
-    <tableColumn id="9" name="Severity" dataDxfId="2"/>
+    <tableColumn id="1" name="#" dataDxfId="9"/>
+    <tableColumn id="2" name="Title" dataDxfId="8"/>
+    <tableColumn id="3" name="Summary" dataDxfId="7"/>
+    <tableColumn id="4" name="Frequency" dataDxfId="6"/>
+    <tableColumn id="5" name="Where(Browser)" dataDxfId="5"/>
+    <tableColumn id="6" name="Steps to Reproduce" dataDxfId="4"/>
+    <tableColumn id="7" name="Actual Result" dataDxfId="3"/>
+    <tableColumn id="8" name="Expected Result" dataDxfId="2"/>
+    <tableColumn id="9" name="Severity" dataDxfId="1"/>
     <tableColumn id="10" name="State" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -594,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,34 +693,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="153" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="153" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="K6" s="3" t="s">
         <v>9</v>
       </c>
@@ -686,7 +761,7 @@
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>

</xml_diff>